<commit_message>
User Data Driven tests added
</commit_message>
<xml_diff>
--- a/PetStoreAPIAutomation/TestData/userData.xlsx
+++ b/PetStoreAPIAutomation/TestData/userData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\Programming\REST_Assured_Framework\PetStoreAPIAutomation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE5D8DBE-6B12-443D-A632-D89B9189A757}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{718810B4-F9C7-4F57-BE21-F81B409172D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12750" yWindow="3210" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4965" yWindow="5355" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -48,15 +48,6 @@
     <t>Phone</t>
   </si>
   <si>
-    <t>testUserOne</t>
-  </si>
-  <si>
-    <t>testUserThree</t>
-  </si>
-  <si>
-    <t>testUserTwo</t>
-  </si>
-  <si>
     <t>Harry</t>
   </si>
   <si>
@@ -75,15 +66,6 @@
     <t>Hamsworth</t>
   </si>
   <si>
-    <t>testone@test.com</t>
-  </si>
-  <si>
-    <t>testtwo@test.com</t>
-  </si>
-  <si>
-    <t>testthre@test.com</t>
-  </si>
-  <si>
     <t>test@1</t>
   </si>
   <si>
@@ -91,6 +73,24 @@
   </si>
   <si>
     <t>test@3</t>
+  </si>
+  <si>
+    <t>testUserFour</t>
+  </si>
+  <si>
+    <t>testUserFive</t>
+  </si>
+  <si>
+    <t>testUserSix</t>
+  </si>
+  <si>
+    <t>testfour@test.com</t>
+  </si>
+  <si>
+    <t>testfive@test.com</t>
+  </si>
+  <si>
+    <t>testsix@test.com</t>
   </si>
 </sst>
 </file>
@@ -445,7 +445,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -484,22 +484,22 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>1010</v>
+        <v>1040</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>19</v>
       </c>
       <c r="G2" s="1">
         <v>12345677</v>
@@ -507,22 +507,22 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>1020</v>
+        <v>1050</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>20</v>
       </c>
       <c r="G3" s="1">
         <v>12345678</v>
@@ -530,22 +530,22 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>1030</v>
+        <v>1060</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="G4" s="1">
         <v>12345679</v>

</xml_diff>